<commit_message>
changes in runner class
</commit_message>
<xml_diff>
--- a/Excel Files/Files.xlsx
+++ b/Excel Files/Files.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="17930" windowHeight="6920"/>
+    <workbookView windowWidth="17930" windowHeight="6920" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login&amp;Usercreation" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="222">
   <si>
     <t>Login page</t>
   </si>
@@ -44,43 +44,43 @@
     <t>First name</t>
   </si>
   <si>
-    <t>Sanjay</t>
-  </si>
-  <si>
-    <t>Asharani</t>
-  </si>
-  <si>
-    <t>Karthik</t>
-  </si>
-  <si>
-    <t>hemavathy</t>
-  </si>
-  <si>
-    <t>Jeeva</t>
-  </si>
-  <si>
-    <t>Maaran</t>
+    <t>Dhoni</t>
+  </si>
+  <si>
+    <t>virat</t>
+  </si>
+  <si>
+    <t>Ravindra</t>
+  </si>
+  <si>
+    <t>Prithvi</t>
+  </si>
+  <si>
+    <t>Kuldeep</t>
+  </si>
+  <si>
+    <t>Sindhu</t>
   </si>
   <si>
     <t>Last name</t>
   </si>
   <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>p</t>
-  </si>
-  <si>
-    <t>n</t>
-  </si>
-  <si>
-    <t>k</t>
-  </si>
-  <si>
-    <t>Balin</t>
-  </si>
-  <si>
-    <t>V</t>
+    <t>MG</t>
+  </si>
+  <si>
+    <t>kohli</t>
+  </si>
+  <si>
+    <t>Jadeja</t>
+  </si>
+  <si>
+    <t>Shaw</t>
+  </si>
+  <si>
+    <t>Yadav</t>
+  </si>
+  <si>
+    <t>Batminton</t>
   </si>
   <si>
     <t>Gender</t>
@@ -95,22 +95,22 @@
     <t>EmailAddress</t>
   </si>
   <si>
-    <t>emarion.shravan@foundtoo.com</t>
-  </si>
-  <si>
-    <t>bronxton.zakery@foundtoo.com</t>
-  </si>
-  <si>
-    <t>davien.stas@foundtoo.com</t>
-  </si>
-  <si>
-    <t>kairav.kadyn@foundtoo.com</t>
-  </si>
-  <si>
-    <t>nelly.wrigley@foundtoo.com</t>
-  </si>
-  <si>
-    <t>maxemiliano.korbyn@foundtoo.com</t>
+    <t>whalen.kieon@foundtoo.com</t>
+  </si>
+  <si>
+    <t>jaylin.chengyu@foundtoo.com</t>
+  </si>
+  <si>
+    <t>legolas.cordero@foundtoo.com</t>
+  </si>
+  <si>
+    <t>camari.lisandro@foundtoo.com</t>
+  </si>
+  <si>
+    <t>jaidin.zorawar@foundtoo.com</t>
+  </si>
+  <si>
+    <t>trinity.colt@foundtoo.com</t>
   </si>
   <si>
     <t>Phone number</t>
@@ -143,342 +143,375 @@
     <t>Profile picture</t>
   </si>
   <si>
-    <t>C:\\Users\\Emarson\\OneDrive - MAVENS I SOFTECH SOLUTIONS PRIVATE LIMITED\\Desktop\\images\\image3.jpg</t>
+    <t>C:\\Users\\Emarson\\OneDrive - MAVENS I SOFTECH SOLUTIONS PRIVATE LIMITED\\Desktop\\images\\image23.jpg</t>
+  </si>
+  <si>
+    <t>C:\\Users\\Emarson\\OneDrive - MAVENS I SOFTECH SOLUTIONS PRIVATE LIMITED\\Desktop\\images\\image24.jpg</t>
+  </si>
+  <si>
+    <t>C:\\Users\\Emarson\\OneDrive - MAVENS I SOFTECH SOLUTIONS PRIVATE LIMITED\\Desktop\\images\\image20.jpg</t>
+  </si>
+  <si>
+    <t>C:\\Users\\Emarson\\OneDrive - MAVENS I SOFTECH SOLUTIONS PRIVATE LIMITED\\Desktop\\images\\image22.jpg</t>
+  </si>
+  <si>
+    <t>C:\\Users\\Emarson\\OneDrive - MAVENS I SOFTECH SOLUTIONS PRIVATE LIMITED\\Desktop\\images\\image29.jpg</t>
+  </si>
+  <si>
+    <t>C:\\Users\\Emarson\\OneDrive - MAVENS I SOFTECH SOLUTIONS PRIVATE LIMITED\\Desktop\\images\\image21.jpg</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Mr</t>
+  </si>
+  <si>
+    <t>Mrs</t>
+  </si>
+  <si>
+    <t>Ms</t>
+  </si>
+  <si>
+    <t>Date of Birth</t>
+  </si>
+  <si>
+    <t>Alternate Contact Number</t>
+  </si>
+  <si>
+    <t>Degree</t>
+  </si>
+  <si>
+    <t>MSD</t>
+  </si>
+  <si>
+    <t>DPT</t>
+  </si>
+  <si>
+    <t>RDH</t>
+  </si>
+  <si>
+    <t>DPM</t>
+  </si>
+  <si>
+    <t>Govt.Id Type</t>
+  </si>
+  <si>
+    <t>Pan card</t>
+  </si>
+  <si>
+    <t>Govt.Id Number</t>
+  </si>
+  <si>
+    <t>Upload Id proof</t>
+  </si>
+  <si>
+    <t>Address Line 1</t>
+  </si>
+  <si>
+    <t>no 278,LIG 2,TNHB colony</t>
+  </si>
+  <si>
+    <t>no1, Monday market, nagercoil</t>
+  </si>
+  <si>
+    <t>no1, Abi flat, S.Kulathur</t>
+  </si>
+  <si>
+    <t>no 32, Miss abragan street, M.G.R nagar</t>
+  </si>
+  <si>
+    <t>no 1, noth new street, kalakadu</t>
+  </si>
+  <si>
+    <t>Address Line 2</t>
+  </si>
+  <si>
+    <t>velachery, Chennai-42</t>
+  </si>
+  <si>
+    <t>Kanyakumary</t>
+  </si>
+  <si>
+    <t>Chennai</t>
+  </si>
+  <si>
+    <t>Tirunelveli</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Delhi</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>East Delhi</t>
+  </si>
+  <si>
+    <t>Pin code</t>
+  </si>
+  <si>
+    <t>Territory</t>
+  </si>
+  <si>
+    <t>Gandhi Nagar</t>
+  </si>
+  <si>
+    <t>About Yourself</t>
+  </si>
+  <si>
+    <t>My name is Dhoni, and I'm an adaptable and experienced hospital administrator. 
+I have 10 years of experience managing hospital operations to ensure that patients and their families receive comprehensive care and support. 
+I value helping others and creating an environment that fosters positive change.</t>
+  </si>
+  <si>
+    <t>My name is Kohli, and I'm an adaptable and experienced hospital administrator. 
+I have 10 years of experience managing hospital operations to ensure that patients and their families receive comprehensive care and support. 
+I value helping others and creating an environment that fosters positive change.</t>
+  </si>
+  <si>
+    <t>My name is Ravindra,32 years old. 
+I was graduated from the Wannan Medical College in Anhui province, my major is clinical medicine. 
+I live in Shanghai from 2007, it’s almost 7years old. 
+I have ever worked in the community health service centre in Chongming and Yangpu district. And now, I’m working in Juquan community, Baoshan district. 
+As a doctor, my motto is “Doing now what patients need”. I spend most of my time to my patients, to help them get out of the pain of disease. 
+However, I’ve never forgot to improve myself with professional medical knowledge. I’ve passed the test of General Intermediate in 2012. 
+And I know that I need to go on study in the future. So today I’m here, to apply the opportunity to attend the medical training in the United States.
+Hope I have this honor.</t>
+  </si>
+  <si>
+    <t>I’m just finishing up nursing school. I’ve got a 3.99 GPA and I received an Outstanding Undergraduate Nursing Student Award for leadership and caring. As a precept nurse at Newark General Hospital, I received frequent commendations from the preceptor for efficiency. I also maintained 95% positive evaluations for patient education. I supervised bedsore prevention on my ward, for which my patients were in the top 98%.</t>
+  </si>
+  <si>
+    <t>In five years, I’d like to be the most valued nurse on your team. I plan to take full advantage of the continuing education reimbursement you offer to expand my skills beyond their current level. I’m skilled in patient education and EHR, which I know you value. There are so many new skills I’d like to gain, including budgeting and training others. I think Cliffton Bluffs Hospital is the perfect place to grow into a better nurse.</t>
+  </si>
+  <si>
+    <t>My name is Sindhu,32 years old. 
+I was graduated from the Wannan Medical College in Anhui province, my major is clinical medicine. 
+I live in Shanghai from 2007, it’s almost 7years old. 
+I have ever worked in the community health service centre in Chongming and Yangpu district. And now, I’m working in Juquan community, Baoshan district. 
+As a doctor, my motto is “Doing now what patients need”. I spend most of my time to my patients, to help them get out of the pain of disease. 
+However, I’ve never forgot to improve myself with professional medical knowledge. I’ve passed the test of General Intermediate in 2012. 
+And I know that I need to go on study in the future. So today I’m here, to apply the opportunity to attend the medical training in the United States.
+Hope I have this honor.</t>
+  </si>
+  <si>
+    <t>Specialty</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Dental cleaning</t>
+  </si>
+  <si>
+    <t>Dermatologist</t>
+  </si>
+  <si>
+    <t>Acupuncturist</t>
+  </si>
+  <si>
+    <t>Registration Year</t>
+  </si>
+  <si>
+    <t>Registration Number</t>
+  </si>
+  <si>
+    <t>Registration Copy</t>
+  </si>
+  <si>
+    <t>Clinic Name</t>
+  </si>
+  <si>
+    <t>Karthik Clinic</t>
+  </si>
+  <si>
+    <t>Hema Clinic</t>
+  </si>
+  <si>
+    <t>Maaran Clinic</t>
+  </si>
+  <si>
+    <t>Clinic Contact Number</t>
+  </si>
+  <si>
+    <t>Clinic Email Address</t>
+  </si>
+  <si>
+    <t>karthik@mail.com</t>
+  </si>
+  <si>
+    <t>hema@mail.com</t>
+  </si>
+  <si>
+    <t>maaran@mail.com</t>
+  </si>
+  <si>
+    <t>Clinic Address</t>
+  </si>
+  <si>
+    <t>Special Skills</t>
+  </si>
+  <si>
+    <t>Patient care</t>
+  </si>
+  <si>
+    <t>Pharmacy name</t>
+  </si>
+  <si>
+    <t>Jeeva pharmacy</t>
+  </si>
+  <si>
+    <t>Pharmacy Contact Number</t>
+  </si>
+  <si>
+    <t>Pharmacy Email address</t>
+  </si>
+  <si>
+    <t>jeeva@mail.com</t>
+  </si>
+  <si>
+    <t>Pharmacy registration no</t>
+  </si>
+  <si>
+    <t>Pharmacy GST no</t>
+  </si>
+  <si>
+    <t>6785ERT6756D</t>
+  </si>
+  <si>
+    <t>Pan card number</t>
+  </si>
+  <si>
+    <t>85ER087656D</t>
+  </si>
+  <si>
+    <t>Pharmacy Address</t>
+  </si>
+  <si>
+    <t>Enquiry page</t>
+  </si>
+  <si>
+    <t>Veteran First Name</t>
+  </si>
+  <si>
+    <t>Rohit</t>
+  </si>
+  <si>
+    <t>Assigned Doctor Names</t>
+  </si>
+  <si>
+    <t>Karthik N</t>
+  </si>
+  <si>
+    <t>Veteran Last Name</t>
+  </si>
+  <si>
+    <t>Sharma</t>
+  </si>
+  <si>
+    <t>Veteran Gender</t>
+  </si>
+  <si>
+    <t>Veteran Email address</t>
+  </si>
+  <si>
+    <t>zandyr.ever@foundtoo.com</t>
+  </si>
+  <si>
+    <t>Veteran Contact Number</t>
+  </si>
+  <si>
+    <t>Veteran Address Line 1</t>
+  </si>
+  <si>
+    <t>278, Anna nagar, mogappiar east</t>
+  </si>
+  <si>
+    <t>Veteran Address Line 2</t>
+  </si>
+  <si>
+    <t>Veteran Country</t>
+  </si>
+  <si>
+    <t>Veteran State/Region</t>
+  </si>
+  <si>
+    <t>Veteran City</t>
+  </si>
+  <si>
+    <t>Veteran Pin code</t>
+  </si>
+  <si>
+    <t>Veteran Territory</t>
+  </si>
+  <si>
+    <t>Family Member First Name</t>
+  </si>
+  <si>
+    <t>Sam</t>
+  </si>
+  <si>
+    <t>Family Member Last Name</t>
+  </si>
+  <si>
+    <t>Curran</t>
+  </si>
+  <si>
+    <t>Family Member Gender</t>
+  </si>
+  <si>
+    <t>Family Member Email address</t>
+  </si>
+  <si>
+    <t>kycen.jexiel@foundtoo.com</t>
+  </si>
+  <si>
+    <t>Family Member Current Address</t>
+  </si>
+  <si>
+    <t>278, Anna nagar, mogappiar east, Chennai -02</t>
+  </si>
+  <si>
+    <t>Family Member Contact Number</t>
+  </si>
+  <si>
+    <t>Family Member Relationship</t>
+  </si>
+  <si>
+    <t>Brother</t>
+  </si>
+  <si>
+    <t>Family Member Notes</t>
+  </si>
+  <si>
+    <t>Accept the enquiry</t>
+  </si>
+  <si>
+    <t>Veteran onboarding form</t>
+  </si>
+  <si>
+    <t>Veteran Profile photo</t>
   </si>
   <si>
     <t>C:\\Users\\Emarson\\OneDrive - MAVENS I SOFTECH SOLUTIONS PRIVATE LIMITED\\Desktop\\images\\image1.jpg</t>
   </si>
   <si>
-    <t>C:\\Users\\Emarson\\OneDrive - MAVENS I SOFTECH SOLUTIONS PRIVATE LIMITED\\Desktop\\images\\image6.jpg</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Emarson\\OneDrive - MAVENS I SOFTECH SOLUTIONS PRIVATE LIMITED\\Desktop\\images\\image7.jpg</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Emarson\\OneDrive - MAVENS I SOFTECH SOLUTIONS PRIVATE LIMITED\\Desktop\\images\\image5.jpg</t>
-  </si>
-  <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>Mr</t>
-  </si>
-  <si>
-    <t>Ms</t>
-  </si>
-  <si>
-    <t>Mrs</t>
-  </si>
-  <si>
-    <t>Date of Birth</t>
-  </si>
-  <si>
-    <t>Alternate Contact Number</t>
-  </si>
-  <si>
-    <t>Degree</t>
-  </si>
-  <si>
-    <t>MSD</t>
-  </si>
-  <si>
-    <t>MD</t>
-  </si>
-  <si>
-    <t>RDH</t>
-  </si>
-  <si>
-    <t>Govt.Id Type</t>
-  </si>
-  <si>
-    <t>Pan card</t>
-  </si>
-  <si>
-    <t>Govt.Id Number</t>
-  </si>
-  <si>
-    <t>Upload Id proof</t>
-  </si>
-  <si>
-    <t>Address Line 1</t>
-  </si>
-  <si>
-    <t>no 278,LIG 2,TNHB colony</t>
-  </si>
-  <si>
-    <t>no1, Monday market, nagercoil</t>
-  </si>
-  <si>
-    <t>no1, Abi flat, S.Kulathur</t>
-  </si>
-  <si>
-    <t>no 32, Miss abragan street, M.G.R nagar</t>
-  </si>
-  <si>
-    <t>no 1, noth new street, kalakadu</t>
-  </si>
-  <si>
-    <t>Address Line 2</t>
-  </si>
-  <si>
-    <t>velachery, Chennai-42</t>
-  </si>
-  <si>
-    <t>Kanyakumary</t>
-  </si>
-  <si>
-    <t>Chennai</t>
-  </si>
-  <si>
-    <t>Tirunelveli</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>India</t>
-  </si>
-  <si>
-    <t>State</t>
-  </si>
-  <si>
-    <t>Delhi</t>
-  </si>
-  <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>East Delhi</t>
-  </si>
-  <si>
-    <t>Pin code</t>
-  </si>
-  <si>
-    <t>Territory</t>
-  </si>
-  <si>
-    <t>Gandhi Nagar</t>
-  </si>
-  <si>
-    <t>About Yourself</t>
-  </si>
-  <si>
-    <t>This is Sanjay.G</t>
-  </si>
-  <si>
-    <t>This is Asharani.P</t>
-  </si>
-  <si>
-    <t>This is Karthik.N</t>
-  </si>
-  <si>
-    <t>This is Hemavathy.K</t>
-  </si>
-  <si>
-    <t>This is Jeevabalin.R</t>
-  </si>
-  <si>
-    <t>This is Maaran V</t>
-  </si>
-  <si>
-    <t>Specialty</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>Urological Surgeon</t>
-  </si>
-  <si>
-    <t>Psychologist</t>
-  </si>
-  <si>
-    <t>Registration Year</t>
-  </si>
-  <si>
-    <t>Registration Number</t>
-  </si>
-  <si>
-    <t>Registration Copy</t>
-  </si>
-  <si>
-    <t>Clinic Name</t>
-  </si>
-  <si>
-    <t>Karthik Clinic</t>
-  </si>
-  <si>
-    <t>Hema Clinic</t>
-  </si>
-  <si>
-    <t>Maaran Clinic</t>
-  </si>
-  <si>
-    <t>Clinic Contact Number</t>
-  </si>
-  <si>
-    <t>Clinic Email Address</t>
-  </si>
-  <si>
-    <t>karthik@mail.com</t>
-  </si>
-  <si>
-    <t>hema@mail.com</t>
-  </si>
-  <si>
-    <t>maaran@mail.com</t>
-  </si>
-  <si>
-    <t>Clinic Address</t>
-  </si>
-  <si>
-    <t>Special Skills</t>
-  </si>
-  <si>
-    <t>Patient Care</t>
-  </si>
-  <si>
-    <t>Pharmacy name</t>
-  </si>
-  <si>
-    <t>Jeeva pharmacy</t>
-  </si>
-  <si>
-    <t>Pharmacy Contact Number</t>
-  </si>
-  <si>
-    <t>Pharmacy Email address</t>
-  </si>
-  <si>
-    <t>jeeva@mail.com</t>
-  </si>
-  <si>
-    <t>Pharmacy registration no</t>
-  </si>
-  <si>
-    <t>Pharmacy GST no</t>
-  </si>
-  <si>
-    <t>6785ERT6756D</t>
-  </si>
-  <si>
-    <t>Pan card number</t>
-  </si>
-  <si>
-    <t>Pharmacy Address</t>
-  </si>
-  <si>
-    <t>Enquiry page</t>
-  </si>
-  <si>
-    <t>Veteran First Name</t>
-  </si>
-  <si>
-    <t>Vinoth</t>
-  </si>
-  <si>
-    <t>Assigned Doctor Names</t>
-  </si>
-  <si>
-    <t>Karthik N</t>
-  </si>
-  <si>
-    <t>Veteran Last Name</t>
-  </si>
-  <si>
-    <t>Gowda</t>
-  </si>
-  <si>
-    <t>Veteran Gender</t>
-  </si>
-  <si>
-    <t>Veteran Email address</t>
-  </si>
-  <si>
-    <t>pinarayivijayan@veteran.com</t>
-  </si>
-  <si>
-    <t>Veteran Contact Number</t>
-  </si>
-  <si>
-    <t>Veteran Address Line 1</t>
-  </si>
-  <si>
-    <t>no 1, south street, perungudi</t>
-  </si>
-  <si>
-    <t>Veteran Address Line 2</t>
-  </si>
-  <si>
-    <t>Veteran Country</t>
-  </si>
-  <si>
-    <t>Veteran State/Region</t>
-  </si>
-  <si>
-    <t>Veteran City</t>
-  </si>
-  <si>
-    <t>Veteran Pin code</t>
-  </si>
-  <si>
-    <t>Veteran Territory</t>
-  </si>
-  <si>
-    <t>Family Member First Name</t>
-  </si>
-  <si>
-    <t>dev</t>
-  </si>
-  <si>
-    <t>Family Member Last Name</t>
-  </si>
-  <si>
-    <t>Patel</t>
-  </si>
-  <si>
-    <t>Family Member Gender</t>
-  </si>
-  <si>
-    <t>Family Member Email address</t>
-  </si>
-  <si>
-    <t>antony@caregiver.com</t>
-  </si>
-  <si>
-    <t>Family Member Current Address</t>
-  </si>
-  <si>
-    <t>no 104, vv street, Chennai</t>
-  </si>
-  <si>
-    <t>Family Member Contact Number</t>
-  </si>
-  <si>
-    <t>Family Member Relationship</t>
-  </si>
-  <si>
-    <t>Brother</t>
-  </si>
-  <si>
-    <t>Family Member Notes</t>
-  </si>
-  <si>
-    <t>Accept the enquiry</t>
-  </si>
-  <si>
-    <t>Veteran onboarding form</t>
-  </si>
-  <si>
-    <t>Veteran Profile photo</t>
-  </si>
-  <si>
-    <t>C:\\Users\\Emarson\\OneDrive - MAVENS I SOFTECH SOLUTIONS PRIVATE LIMITED\\Desktop\\images\\image11.jpeg</t>
-  </si>
-  <si>
     <t>Family member Profile photo</t>
   </si>
   <si>
+    <t>C:\\Users\\Emarson\\OneDrive - MAVENS I SOFTECH SOLUTIONS PRIVATE LIMITED\\Desktop\\images\\image2.jpg</t>
+  </si>
+  <si>
     <t>Respective Police Station</t>
   </si>
   <si>
@@ -554,7 +587,7 @@
     <t>Comorbidities</t>
   </si>
   <si>
-    <t>Blood Pressure</t>
+    <t>Thyroid disorders</t>
   </si>
   <si>
     <t>From Duration</t>
@@ -566,7 +599,7 @@
     <t>History of Comorbidities</t>
   </si>
   <si>
-    <t>Test</t>
+    <t>On 2016, Thyroid disorders disease, so my blood pressure also increased</t>
   </si>
   <si>
     <t>Any Hospitalization in last 5 years? When?</t>
@@ -581,6 +614,9 @@
     <t>Any Hospitalization in last 5 years? History</t>
   </si>
   <si>
+    <t>on 2018, i was hospitalized on chennai govt hospital.</t>
+  </si>
+  <si>
     <t>Any Heart disease? When?</t>
   </si>
   <si>
@@ -590,6 +626,9 @@
     <t>Any Heart disease? History</t>
   </si>
   <si>
+    <t>2020, heart disease with low BP</t>
+  </si>
+  <si>
     <t>Any kidney disease? When?</t>
   </si>
   <si>
@@ -599,6 +638,9 @@
     <t>Any kidney disease? History</t>
   </si>
   <si>
+    <t>i was hospitalized with kidney stone</t>
+  </si>
+  <si>
     <t>Any Cancer History? When?</t>
   </si>
   <si>
@@ -617,7 +659,7 @@
     <t>Medicine Name</t>
   </si>
   <si>
-    <t>Dolo</t>
+    <t>Asprin</t>
   </si>
   <si>
     <t>Dosage</t>
@@ -629,7 +671,7 @@
     <t>Name of the Insurance carrier</t>
   </si>
   <si>
-    <t>ICICI Prudential</t>
+    <t>Life insurance corporation of india</t>
   </si>
   <si>
     <t>Policy Number</t>
@@ -641,7 +683,7 @@
     <t>Insurance Email address</t>
   </si>
   <si>
-    <t>karthik@gmail.com</t>
+    <t>kabil@gmail.com</t>
   </si>
   <si>
     <t>Copy of policy</t>
@@ -656,7 +698,7 @@
     <t>Insurance Address</t>
   </si>
   <si>
-    <t>linken.sahel@foundtoo.com</t>
+    <t>Madhurai</t>
   </si>
 </sst>
 </file>
@@ -664,12 +706,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -687,17 +729,21 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF000000"/>
+      <color rgb="FF202124"/>
       <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF333333"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10.05"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <charset val="134"/>
     </font>
     <font>
       <u/>
@@ -728,46 +774,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -783,10 +791,56 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -798,16 +852,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -829,14 +875,22 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -857,7 +911,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -869,7 +959,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -881,73 +1073,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -959,85 +1091,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1103,6 +1157,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1114,26 +1186,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1168,15 +1220,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1200,20 +1243,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1223,134 +1277,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1378,11 +1432,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1393,9 +1444,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1405,10 +1462,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="7" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="7" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1735,39 +1792,39 @@
   <sheetPr/>
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="22.5454545454545" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="43.9090909090909" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="44.5454545454545" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="44.4545454545455" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" style="1" width="48.0" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="44.3636363636364" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="41.0909090909091" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" width="44.1818181818182" collapsed="false"/>
+    <col min="1" max="1" width="22.5454545454545" customWidth="1"/>
+    <col min="2" max="2" width="43.9090909090909" customWidth="1"/>
+    <col min="3" max="3" width="44.5454545454545" customWidth="1"/>
+    <col min="4" max="4" width="44.4545454545455" customWidth="1"/>
+    <col min="5" max="5" width="48" style="1" customWidth="1"/>
+    <col min="6" max="6" width="44.3636363636364" customWidth="1"/>
+    <col min="7" max="7" width="41.0909090909091" customWidth="1"/>
+    <col min="8" max="8" width="44.1818181818182" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="17"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="18"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="19" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="7"/>
@@ -1781,7 +1838,7 @@
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="19" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="7"/>
@@ -1795,7 +1852,7 @@
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="19" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="7"/>
@@ -1830,7 +1887,7 @@
       <c r="D6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="15" t="s">
         <v>12</v>
       </c>
       <c r="F6" s="8" t="s">
@@ -1873,7 +1930,7 @@
         <v>23</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>23</v>
@@ -1882,10 +1939,10 @@
         <v>24</v>
       </c>
       <c r="F8" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="8" t="s">
         <v>24</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>23</v>
       </c>
       <c r="H8" s="7"/>
     </row>
@@ -1894,7 +1951,7 @@
         <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>213</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
         <v>27</v>
@@ -1918,7 +1975,7 @@
         <v>32</v>
       </c>
       <c r="B10" s="8">
-        <v>9878576500</v>
+        <v>9876543210</v>
       </c>
       <c r="C10" s="8">
         <v>8867583456</v>
@@ -1941,7 +1998,7 @@
       <c r="A11" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="20" t="s">
         <v>34</v>
       </c>
       <c r="C11" s="8" t="s">
@@ -1989,32 +2046,32 @@
       <c r="A13" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="F13" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="G13" s="11" t="s">
-        <v>44</v>
+      <c r="G13" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="H13" s="7"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>49</v>
@@ -2023,10 +2080,10 @@
         <v>50</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G14" s="8" t="s">
         <v>50</v>
@@ -2035,31 +2092,31 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B15" s="12">
+        <v>52</v>
+      </c>
+      <c r="B15" s="11">
         <v>37048</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C15" s="11">
         <v>36069</v>
       </c>
-      <c r="D15" s="12">
+      <c r="D15" s="11">
         <v>31263</v>
       </c>
-      <c r="E15" s="12">
+      <c r="E15" s="11">
         <v>37166</v>
       </c>
-      <c r="F15" s="12">
+      <c r="F15" s="11">
         <v>36956</v>
       </c>
-      <c r="G15" s="12">
+      <c r="G15" s="11">
         <v>31263</v>
       </c>
       <c r="H15" s="7"/>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B16" s="8">
         <v>87865645432</v>
@@ -2083,55 +2140,55 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="H17" s="7"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H18" s="7"/>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B19" s="8">
         <v>8796754653</v>
@@ -2155,151 +2212,151 @@
     </row>
     <row r="20" ht="43.5" spans="1:8">
       <c r="A20" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B20" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="E20" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="F20" s="11" t="s">
+      <c r="F20" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="G20" s="11" t="s">
-        <v>44</v>
+      <c r="G20" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="H20" s="7"/>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="5" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F21" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="G21" s="8" t="s">
         <v>66</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>64</v>
       </c>
       <c r="H21" s="7"/>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="5" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H22" s="7"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="5" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H23" s="7"/>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="H24" s="7"/>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="H25" s="7"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B26" s="8">
         <v>657846</v>
@@ -2323,85 +2380,85 @@
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="5" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="H27" s="7"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" ht="319" spans="1:8">
       <c r="A28" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="C28" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="B28" s="10" t="s">
         <v>84</v>
       </c>
+      <c r="C28" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>86</v>
+      </c>
       <c r="E28" s="8" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G28" s="8" t="s">
-        <v>87</v>
+        <v>88</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>89</v>
       </c>
       <c r="H28" s="7"/>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B29" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="C29" s="20" t="s">
-        <v>89</v>
+        <v>90</v>
+      </c>
+      <c r="B29" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C29" s="21" t="s">
+        <v>91</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="H29" s="7"/>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B30" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="C30" s="20" t="s">
-        <v>89</v>
+        <v>95</v>
+      </c>
+      <c r="B30" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C30" s="21" t="s">
+        <v>91</v>
       </c>
       <c r="D30" s="8">
         <v>2016</v>
@@ -2419,13 +2476,13 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="B31" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="C31" s="20" t="s">
-        <v>89</v>
+        <v>96</v>
+      </c>
+      <c r="B31" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C31" s="21" t="s">
+        <v>91</v>
       </c>
       <c r="D31" s="8">
         <v>7685943654</v>
@@ -2443,61 +2500,61 @@
     </row>
     <row r="32" ht="43.5" spans="1:8">
       <c r="A32" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="B32" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="C32" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="D32" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="B32" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C32" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="D32" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E32" s="11" t="s">
+      <c r="E32" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="F32" s="11" t="s">
+      <c r="F32" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="G32" s="11" t="s">
-        <v>44</v>
+      <c r="G32" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="H32" s="7"/>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="B33" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="C33" s="20" t="s">
-        <v>89</v>
+        <v>98</v>
+      </c>
+      <c r="B33" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C33" s="21" t="s">
+        <v>91</v>
       </c>
       <c r="D33" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="G33" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="H33" s="7"/>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="B34" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="C34" s="20" t="s">
-        <v>89</v>
+        <v>102</v>
+      </c>
+      <c r="B34" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C34" s="21" t="s">
+        <v>91</v>
       </c>
       <c r="D34" s="8">
         <v>8965434567</v>
@@ -2506,7 +2563,7 @@
         <v>8965434767</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="G34" s="8">
         <v>8965434167</v>
@@ -2515,241 +2572,241 @@
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="B35" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="C35" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="D35" s="18" t="s">
-        <v>101</v>
-      </c>
-      <c r="E35" s="10" t="s">
-        <v>102</v>
+        <v>103</v>
+      </c>
+      <c r="B35" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C35" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="D35" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="E35" s="15" t="s">
+        <v>105</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="G35" s="18" t="s">
-        <v>103</v>
+        <v>91</v>
+      </c>
+      <c r="G35" s="19" t="s">
+        <v>106</v>
       </c>
       <c r="H35" s="7"/>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="B36" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="C36" s="20" t="s">
-        <v>89</v>
+        <v>107</v>
+      </c>
+      <c r="B36" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C36" s="21" t="s">
+        <v>91</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H36" s="7"/>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="B37" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="C37" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="D37" s="20" t="s">
-        <v>89</v>
+        <v>108</v>
+      </c>
+      <c r="B37" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C37" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="D37" s="21" t="s">
+        <v>91</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="G37" s="20" t="s">
-        <v>89</v>
+        <v>91</v>
+      </c>
+      <c r="G37" s="21" t="s">
+        <v>91</v>
       </c>
       <c r="H37" s="7"/>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="B38" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="C38" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="D38" s="20" t="s">
-        <v>89</v>
+        <v>110</v>
+      </c>
+      <c r="B38" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C38" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="D38" s="21" t="s">
+        <v>91</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="G38" s="20" t="s">
-        <v>89</v>
+        <v>111</v>
+      </c>
+      <c r="G38" s="21" t="s">
+        <v>91</v>
       </c>
       <c r="H38" s="7"/>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B39" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="C39" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="D39" s="20" t="s">
-        <v>89</v>
+        <v>112</v>
+      </c>
+      <c r="B39" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C39" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="D39" s="21" t="s">
+        <v>91</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F39" s="8">
         <v>9878675473</v>
       </c>
-      <c r="G39" s="20" t="s">
-        <v>89</v>
+      <c r="G39" s="21" t="s">
+        <v>91</v>
       </c>
       <c r="H39" s="7"/>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="B40" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="C40" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="D40" s="20" t="s">
-        <v>89</v>
+        <v>113</v>
+      </c>
+      <c r="B40" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C40" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="D40" s="21" t="s">
+        <v>91</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="F40" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="G40" s="20" t="s">
-        <v>89</v>
+        <v>91</v>
+      </c>
+      <c r="F40" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="G40" s="21" t="s">
+        <v>91</v>
       </c>
       <c r="H40" s="7"/>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="B41" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="C41" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="D41" s="20" t="s">
-        <v>89</v>
+        <v>115</v>
+      </c>
+      <c r="B41" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C41" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="D41" s="21" t="s">
+        <v>91</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F41" s="8">
         <v>8796754364</v>
       </c>
-      <c r="G41" s="20" t="s">
-        <v>89</v>
+      <c r="G41" s="21" t="s">
+        <v>91</v>
       </c>
       <c r="H41" s="7"/>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B42" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="C42" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="D42" s="20" t="s">
-        <v>89</v>
+        <v>116</v>
+      </c>
+      <c r="B42" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C42" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="D42" s="21" t="s">
+        <v>91</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="G42" s="20" t="s">
-        <v>89</v>
+        <v>117</v>
+      </c>
+      <c r="G42" s="21" t="s">
+        <v>91</v>
       </c>
       <c r="H42" s="7"/>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="B43" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="C43" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="D43" s="20" t="s">
-        <v>89</v>
+        <v>118</v>
+      </c>
+      <c r="B43" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C43" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="D43" s="21" t="s">
+        <v>91</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="G43" s="20" t="s">
-        <v>89</v>
+        <v>119</v>
+      </c>
+      <c r="G43" s="21" t="s">
+        <v>91</v>
       </c>
       <c r="H43" s="7"/>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="B44" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="C44" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="D44" s="20" t="s">
-        <v>89</v>
+        <v>120</v>
+      </c>
+      <c r="B44" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C44" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="D44" s="21" t="s">
+        <v>91</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="G44" s="20" t="s">
-        <v>89</v>
+        <v>72</v>
+      </c>
+      <c r="G44" s="21" t="s">
+        <v>91</v>
       </c>
       <c r="H44" s="7"/>
     </row>
@@ -2759,14 +2816,9 @@
     <mergeCell ref="A5:H5"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId9" display="Welldercare@1"/>
-    <hyperlink ref="B3" r:id="rId10" display="prakash.dhanapalan@mavens-i.com"/>
-    <hyperlink ref="B2" r:id="rId11" display="http://65.108.222.73/#/en/login" tooltip="http://65.108.222.73/#/en/login"/>
-    <hyperlink ref="B9" r:id="rId12" display="emarion.shravan@foundtoo.com" tooltip="mailto:sanjay@channelpartner.com"/>
-    <hyperlink ref="D35" r:id="rId13" display="karthik@mail.com"/>
-    <hyperlink ref="E35" r:id="rId14" display="hema@mail.com"/>
-    <hyperlink ref="F40" r:id="rId15" display="jeeva@mail.com"/>
-    <hyperlink ref="G35" r:id="rId16" display="maaran@mail.com" tooltip="mailto:maaran@mail.com"/>
+    <hyperlink ref="B4" r:id="rId1" display="Welldercare@1"/>
+    <hyperlink ref="B3" r:id="rId2" display="prakash.dhanapalan@mavens-i.com"/>
+    <hyperlink ref="B2" r:id="rId3" display="http://65.108.222.73/#/en/login" tooltip="http://65.108.222.73/#/en/login"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -2778,23 +2830,23 @@
   <sheetPr/>
   <dimension ref="A1:F69"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="36.0909090909091" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" style="1" width="44.6363636363636" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="26.4545454545455" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="44.2727272727273" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="14.0" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" style="2" width="17.3636363636364" collapsed="false"/>
+    <col min="1" max="1" width="36.0909090909091" customWidth="1"/>
+    <col min="2" max="2" width="44.6363636363636" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26.4545454545455" customWidth="1"/>
+    <col min="4" max="4" width="44.2727272727273" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="17.3636363636364" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="3" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="3"/>
@@ -2804,26 +2856,26 @@
     </row>
     <row r="2" ht="15.5" spans="1:6">
       <c r="A2" s="5" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
     </row>
     <row r="3" ht="15.5" spans="1:6">
       <c r="A3" s="5" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="7"/>
@@ -2832,7 +2884,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="5" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>23</v>
@@ -2844,10 +2896,10 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="5" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
@@ -2856,10 +2908,10 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="5" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B6" s="8">
-        <v>9989000011</v>
+        <v>9989545436</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
@@ -2868,10 +2920,10 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="5" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -2880,10 +2932,10 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="5" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
@@ -2892,10 +2944,10 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="5" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
@@ -2904,10 +2956,10 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="5" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
@@ -2916,10 +2968,10 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
@@ -2928,10 +2980,10 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="5" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="B12" s="8">
-        <v>654783</v>
+        <v>675342</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
@@ -2940,22 +2992,22 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="5" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" ht="15.5" spans="1:6">
       <c r="A14" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>137</v>
+        <v>140</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>141</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
@@ -2964,10 +3016,10 @@
     </row>
     <row r="15" ht="15.5" spans="1:6">
       <c r="A15" s="5" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
@@ -2976,7 +3028,7 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="5" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>23</v>
@@ -2988,10 +3040,10 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>142</v>
+        <v>145</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>146</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
@@ -3000,10 +3052,10 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="5" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
@@ -3012,10 +3064,10 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="5" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B19" s="8">
-        <v>9989000012</v>
+        <v>9989987643</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
@@ -3024,10 +3076,10 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="5" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
@@ -3036,10 +3088,10 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="5" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
@@ -3048,7 +3100,7 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="3" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -3058,61 +3110,61 @@
     </row>
     <row r="23" ht="43.5" spans="1:6">
       <c r="A23" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>152</v>
+        <v>155</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>156</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>152</v>
+        <v>157</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>158</v>
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>50</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B25" s="12">
+        <v>52</v>
+      </c>
+      <c r="B25" s="11">
         <v>29498</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B26" s="8">
         <v>8796543233</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D26" s="8">
         <v>8790660086</v>
@@ -3122,31 +3174,31 @@
     </row>
     <row r="27" ht="43.5" spans="1:6">
       <c r="A27" s="5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>152</v>
+        <v>62</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>158</v>
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B28" s="8">
         <v>8790660586</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D28" s="12">
+        <v>52</v>
+      </c>
+      <c r="D28" s="11">
         <v>29498</v>
       </c>
       <c r="E28" s="7"/>
@@ -3154,13 +3206,13 @@
     </row>
     <row r="29" ht="43.5" spans="1:6">
       <c r="A29" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B29" s="11" t="s">
-        <v>152</v>
+        <v>62</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>156</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="D29" s="1">
         <v>9878675843</v>
@@ -3170,13 +3222,13 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="5" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="B30" s="8">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="D30" s="8">
         <v>678564</v>
@@ -3186,13 +3238,13 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="5" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="B31" s="8">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D31" s="8">
         <v>9674563452</v>
@@ -3202,61 +3254,61 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="5" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>159</v>
-      </c>
-      <c r="C32" s="13" t="s">
-        <v>160</v>
+        <v>164</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>165</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="E32" s="7"/>
       <c r="F32" s="7"/>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="5" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="B33" s="8">
         <v>36.8</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="5" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="B34" s="8">
         <v>78</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="5" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
@@ -3264,13 +3316,13 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="5" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="B36" s="8">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="D36" s="8"/>
       <c r="E36" s="7"/>
@@ -3278,13 +3330,13 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="5" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="B37" s="8">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
@@ -3292,10 +3344,10 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="5" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="B38" s="8">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
@@ -3304,10 +3356,10 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="5" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="B39" s="8">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
@@ -3316,10 +3368,10 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="5" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="B40" s="8">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
@@ -3328,10 +3380,10 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>179</v>
+        <v>183</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>184</v>
       </c>
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
@@ -3340,7 +3392,7 @@
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="5" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="B42" s="8">
         <v>2016</v>
@@ -3352,7 +3404,7 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="5" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="B43" s="8">
         <v>2020</v>
@@ -3362,12 +3414,12 @@
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" ht="29" spans="1:6">
       <c r="A44" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>183</v>
+        <v>187</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>188</v>
       </c>
       <c r="C44" s="7"/>
       <c r="D44" s="7"/>
@@ -3376,7 +3428,7 @@
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="5" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="B45" s="8">
         <v>2018</v>
@@ -3388,10 +3440,10 @@
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="5" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
@@ -3400,10 +3452,10 @@
     </row>
     <row r="47" ht="43.5" spans="1:6">
       <c r="A47" s="14" t="s">
-        <v>186</v>
-      </c>
-      <c r="B47" s="11" t="s">
-        <v>152</v>
+        <v>191</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>156</v>
       </c>
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
@@ -3412,10 +3464,10 @@
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="5" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>183</v>
+        <v>193</v>
       </c>
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
@@ -3424,7 +3476,7 @@
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="5" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="B49" s="8">
         <v>2020</v>
@@ -3436,10 +3488,10 @@
     </row>
     <row r="50" spans="1:6">
       <c r="A50" s="5" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C50" s="7"/>
       <c r="D50" s="7"/>
@@ -3448,10 +3500,10 @@
     </row>
     <row r="51" spans="1:6">
       <c r="A51" s="5" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>183</v>
+        <v>197</v>
       </c>
       <c r="C51" s="7"/>
       <c r="D51" s="7"/>
@@ -3460,7 +3512,7 @@
     </row>
     <row r="52" spans="1:6">
       <c r="A52" s="5" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="B52" s="8">
         <v>2013</v>
@@ -3472,10 +3524,10 @@
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="5" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C53" s="7"/>
       <c r="D53" s="7"/>
@@ -3484,10 +3536,10 @@
     </row>
     <row r="54" spans="1:6">
       <c r="A54" s="5" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>183</v>
+        <v>201</v>
       </c>
       <c r="C54" s="7"/>
       <c r="D54" s="7"/>
@@ -3496,7 +3548,7 @@
     </row>
     <row r="55" spans="1:6">
       <c r="A55" s="5" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="B55" s="8">
         <v>2018</v>
@@ -3508,10 +3560,10 @@
     </row>
     <row r="56" spans="1:6">
       <c r="A56" s="5" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C56" s="7"/>
       <c r="D56" s="7"/>
@@ -3520,10 +3572,10 @@
     </row>
     <row r="57" spans="1:6">
       <c r="A57" s="5" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>183</v>
+        <v>193</v>
       </c>
       <c r="C57" s="7"/>
       <c r="D57" s="7"/>
@@ -3532,10 +3584,10 @@
     </row>
     <row r="58" spans="1:6">
       <c r="A58" s="5" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="C58" s="7"/>
       <c r="D58" s="7"/>
@@ -3544,10 +3596,10 @@
     </row>
     <row r="59" spans="1:6">
       <c r="A59" s="5" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="C59" s="7"/>
       <c r="D59" s="7"/>
@@ -3556,10 +3608,10 @@
     </row>
     <row r="60" spans="1:6">
       <c r="A60" s="5" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="B60" s="8">
-        <v>600</v>
+        <v>250</v>
       </c>
       <c r="C60" s="7"/>
       <c r="D60" s="7"/>
@@ -3568,7 +3620,7 @@
     </row>
     <row r="61" spans="1:6">
       <c r="A61" s="5" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="B61" s="8">
         <v>2022</v>
@@ -3580,10 +3632,10 @@
     </row>
     <row r="62" spans="1:6">
       <c r="A62" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="B62" s="8" t="s">
-        <v>204</v>
+        <v>211</v>
+      </c>
+      <c r="B62" s="13" t="s">
+        <v>212</v>
       </c>
       <c r="C62" s="7"/>
       <c r="D62" s="7"/>
@@ -3592,7 +3644,7 @@
     </row>
     <row r="63" spans="1:6">
       <c r="A63" s="5" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="B63" s="8">
         <v>8765784145</v>
@@ -3604,7 +3656,7 @@
     </row>
     <row r="64" spans="1:6">
       <c r="A64" s="5" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="B64" s="8">
         <v>60000000</v>
@@ -3616,10 +3668,10 @@
     </row>
     <row r="65" spans="1:6">
       <c r="A65" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="B65" s="10" t="s">
-        <v>208</v>
+        <v>215</v>
+      </c>
+      <c r="B65" s="15" t="s">
+        <v>216</v>
       </c>
       <c r="C65" s="7"/>
       <c r="D65" s="7"/>
@@ -3628,10 +3680,10 @@
     </row>
     <row r="66" ht="43.5" spans="1:6">
       <c r="A66" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="B66" s="11" t="s">
-        <v>152</v>
+        <v>217</v>
+      </c>
+      <c r="B66" s="10" t="s">
+        <v>156</v>
       </c>
       <c r="C66" s="7"/>
       <c r="D66" s="7"/>
@@ -3640,9 +3692,9 @@
     </row>
     <row r="67" spans="1:6">
       <c r="A67" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="B67" s="12">
+        <v>218</v>
+      </c>
+      <c r="B67" s="11">
         <v>47636</v>
       </c>
       <c r="C67" s="7"/>
@@ -3652,10 +3704,10 @@
     </row>
     <row r="68" spans="1:6">
       <c r="A68" s="5" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="B68" s="8">
-        <v>8796543234</v>
+        <v>8767543543</v>
       </c>
       <c r="C68" s="7"/>
       <c r="D68" s="7"/>
@@ -3664,10 +3716,10 @@
     </row>
     <row r="69" spans="1:6">
       <c r="A69" s="5" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>70</v>
+        <v>221</v>
       </c>
       <c r="C69" s="7"/>
       <c r="D69" s="7"/>
@@ -3680,7 +3732,7 @@
     <mergeCell ref="A22:F22"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B65" r:id="rId2" display="karthik@gmail.com"/>
+    <hyperlink ref="B65" r:id="rId1" display="kabil@gmail.com" tooltip="mailto:kabil@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>